<commit_message>
Add pivot field now doesn't have subtotal by default.
That is not how Excel does it (it has automatic subtotal), but that is how
ClosedXML does it. Also, we have method to add subtotal, but not remove it.
So not having anything gives users most options.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTable/Create/Add_one_column_and_one_value.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTable/Create/Add_one_column_and_one_value.xlsx
@@ -90,10 +90,9 @@
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Test" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" outline="1">
   <location ref="A1" firstHeaderRow="0" firstDataRow="0" firstDataCol="0"/>
   <pivotFields count="2">
-    <pivotField name="A" axis="axisCol" showAll="0">
-      <items count="2">
+    <pivotField name="A" axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="1">
         <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>

</xml_diff>